<commit_message>
Add image to ressource.resx
refactoty image and put it in the application ressources
</commit_message>
<xml_diff>
--- a/TestsSaveExcel/BenGabrant.xlsx
+++ b/TestsSaveExcel/BenGabrant.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <x:si>
     <x:t>MEMORY CARDS</x:t>
   </x:si>
@@ -79,7 +79,7 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>Abstrait</x:t>
+    <x:t>Images</x:t>
   </x:si>
   <x:si>
     <x:t>24</x:t>
@@ -101,9 +101,6 @@
   </x:si>
   <x:si>
     <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NaN</x:t>
   </x:si>
   <x:si>
     <x:t>6</x:t>
@@ -1950,7 +1947,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B6" s="83">
-        <x:v>43794</x:v>
+        <x:v>43802</x:v>
       </x:c>
       <x:c r="C6" s="83" t="s"/>
       <x:c r="D6" s="83" t="s"/>
@@ -1969,7 +1966,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B7" s="85">
-        <x:v>43794.6914236111</x:v>
+        <x:v>43802.5119444444</x:v>
       </x:c>
       <x:c r="C7" s="85" t="s"/>
       <x:c r="D7" s="85" t="s"/>
@@ -2100,13 +2097,13 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="F13" s="23" t="n">
-        <x:v>12</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G13" s="23" t="n">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="H13" s="24" t="n">
-        <x:v>83.33</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="I13" s="75" t="s"/>
       <x:c r="J13" s="75" t="s"/>
@@ -2131,7 +2128,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="F14" s="98" t="n">
-        <x:v>2</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G14" s="98" t="n">
         <x:v>0</x:v>
@@ -2162,7 +2159,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="F15" s="23" t="n">
-        <x:v>2</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G15" s="23" t="n">
         <x:v>0</x:v>
@@ -2193,13 +2190,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="F16" s="98" t="n">
-        <x:v>2</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G16" s="98" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="H16" s="99" t="n">
-        <x:v>50</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="I16" s="75" t="s"/>
       <x:c r="J16" s="75" t="s"/>
@@ -2224,13 +2221,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="F17" s="23" t="n">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G17" s="23" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="H17" s="24" t="s">
-        <x:v>27</x:v>
+      <x:c r="H17" s="24" t="n">
+        <x:v>100</x:v>
       </x:c>
       <x:c r="I17" s="75" t="s"/>
       <x:c r="J17" s="75" t="s"/>
@@ -2240,7 +2237,7 @@
     </x:row>
     <x:row r="18" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A18" s="100" t="s">
-        <x:v>28</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B18" s="101" t="s">
         <x:v>19</x:v>
@@ -2255,7 +2252,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="F18" s="102" t="n">
-        <x:v>1</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="G18" s="102" t="n">
         <x:v>0</x:v>
@@ -2286,10 +2283,10 @@
     </x:row>
     <x:row r="20" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A20" s="104" t="s">
-        <x:v>29</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B20" s="78" t="n">
-        <x:v>3.17</x:v>
+        <x:v>13.67</x:v>
       </x:c>
       <x:c r="C20" s="78" t="s"/>
       <x:c r="D20" s="78" t="s"/>
@@ -2305,10 +2302,10 @@
     </x:row>
     <x:row r="21" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A21" s="74" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B21" s="81" t="n">
-        <x:v>0.5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="C21" s="81" t="s"/>
       <x:c r="D21" s="81" t="s"/>
@@ -2324,10 +2321,10 @@
     </x:row>
     <x:row r="22" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A22" s="104" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B22" s="78" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B22" s="78" t="n">
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C22" s="78" t="s"/>
       <x:c r="D22" s="78" t="s"/>
@@ -2358,7 +2355,7 @@
     </x:row>
     <x:row r="24" spans="1:1025" s="70" customFormat="1" ht="19.4" customHeight="1" outlineLevel="0">
       <x:c r="A24" s="105" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B24" s="106" t="s"/>
       <x:c r="C24" s="106" t="s"/>
@@ -2390,13 +2387,13 @@
     </x:row>
     <x:row r="26" spans="1:1025" s="70" customFormat="1" ht="15" customHeight="1" outlineLevel="0">
       <x:c r="A26" s="108" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B26" s="109" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C26" s="110" t="s">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D26" s="111" t="s"/>
       <x:c r="E26" s="110" t="s">
@@ -2409,7 +2406,7 @@
       <x:c r="H26" s="112" t="s"/>
       <x:c r="I26" s="113" t="s"/>
       <x:c r="J26" s="114" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="K26" s="115" t="s"/>
       <x:c r="L26" s="112" t="s"/>
@@ -2419,22 +2416,22 @@
       <x:c r="A27" s="116" t="s"/>
       <x:c r="B27" s="117" t="s"/>
       <x:c r="C27" s="118" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D27" s="118" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="D27" s="118" t="s">
+      <x:c r="E27" s="118" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F27" s="118" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G27" s="118" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="E27" s="118" t="s">
+      <x:c r="H27" s="119" t="s">
         <x:v>36</x:v>
-      </x:c>
-      <x:c r="F27" s="118" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="G27" s="118" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="H27" s="119" t="s">
-        <x:v>37</x:v>
       </x:c>
       <x:c r="I27" s="120" t="s"/>
       <x:c r="J27" s="121" t="s">
@@ -2450,7 +2447,7 @@
     </x:row>
     <x:row r="28" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A28" s="124" t="s">
-        <x:v>39</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B28" s="23" t="n">
         <x:v>1</x:v>
@@ -2663,7 +2660,7 @@
     <x:row r="34" spans="1:1025" s="70" customFormat="1" ht="13.8" customHeight="1" outlineLevel="0">
       <x:c r="A34" s="132" t="s"/>
       <x:c r="B34" s="60" t="s">
-        <x:v>40</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C34" s="61" t="n">
         <x:v>18</x:v>

</xml_diff>